<commit_message>
Added all the test cases
</commit_message>
<xml_diff>
--- a/docs/Lab3/InClass/Lab03_WBT_Form.xlsx
+++ b/docs/Lab3/InClass/Lab03_WBT_Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrei\SSVV\MavenApp\docs\Lab3\InClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123940C9-56BB-43BF-B75C-1F9B0D0CA230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E35801B-042E-44AB-BA8B-FFB18E060952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="947" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13428" yWindow="2736" windowWidth="17280" windowHeight="8964" tabRatio="947" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem" sheetId="5" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="67">
   <si>
     <t>Statement</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>1,2,3,4,5,6,8,9,11</t>
-  </si>
-  <si>
-    <t>not null</t>
   </si>
   <si>
     <t>Remarks</t>
@@ -320,7 +317,7 @@
     <t>Req_b)</t>
   </si>
   <si>
-    <t>not yet</t>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -868,6 +865,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -877,20 +889,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -926,18 +935,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1574,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="M3:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
@@ -1678,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1700,26 +1697,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="36" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
       <c r="X1" s="23" t="s">
         <v>16</v>
       </c>
@@ -1732,53 +1729,53 @@
     </row>
     <row r="2" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41" t="s">
+      <c r="D2" s="37"/>
+      <c r="E2" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="42"/>
+      <c r="F2" s="39"/>
       <c r="G2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43" t="s">
+      <c r="I2" s="40"/>
+      <c r="J2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43" t="s">
+      <c r="K2" s="40"/>
+      <c r="L2" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43" t="s">
+      <c r="M2" s="40"/>
+      <c r="N2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43" t="s">
+      <c r="O2" s="40"/>
+      <c r="P2" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="37">
+      <c r="Q2" s="40"/>
+      <c r="R2" s="42">
         <v>1</v>
       </c>
-      <c r="S2" s="37">
+      <c r="S2" s="42">
         <v>2</v>
       </c>
-      <c r="T2" s="37">
+      <c r="T2" s="42">
         <v>3</v>
       </c>
-      <c r="U2" s="37">
+      <c r="U2" s="42">
         <v>4</v>
       </c>
-      <c r="V2" s="37">
+      <c r="V2" s="42">
         <v>5</v>
       </c>
-      <c r="W2" s="37">
+      <c r="W2" s="42">
         <v>6</v>
       </c>
       <c r="X2" s="23"/>
@@ -1838,12 +1835,12 @@
       <c r="Q3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
       <c r="X3" s="23" t="s">
         <v>32</v>
       </c>
@@ -2445,42 +2442,22 @@
       <c r="AD15" s="23"/>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B16" s="15">
-        <v>13</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>43</v>
-      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="14"/>
-      <c r="G16" s="18" t="s">
-        <v>44</v>
-      </c>
+      <c r="G16" s="18"/>
       <c r="H16" s="20"/>
-      <c r="I16" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="K16" s="20"/>
       <c r="L16" s="20"/>
-      <c r="M16" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="M16" s="20"/>
       <c r="N16" s="20"/>
-      <c r="O16" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="O16" s="20"/>
       <c r="P16" s="20"/>
-      <c r="Q16" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="Q16" s="20"/>
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
       <c r="T16" s="22"/>
@@ -2559,34 +2536,41 @@
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C23" s="36" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="C23" s="39" t="s">
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C24" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-    </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="C24" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C25" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="C24:G24"/>
     <mergeCell ref="C2:D2"/>
@@ -2597,13 +2581,6 @@
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R1:W1"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2614,8 +2591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2625,110 +2602,113 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="31"/>
+    </row>
+    <row r="5" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="31"/>
-    </row>
-    <row r="5" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="56" t="s">
+      <c r="C5" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="D5" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="E5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="F5" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="G5" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="H5" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="I5" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="44" t="s">
+      <c r="L5" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="44" t="s">
+      <c r="M5" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="M5" s="47" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="6" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="56"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="48"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="52"/>
     </row>
     <row r="7" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="27">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="28">
+        <v>1</v>
+      </c>
+      <c r="H7" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="27">
-        <f>SUM(D7:E7)</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29" t="s">
-        <v>32</v>
-      </c>
       <c r="I7" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" s="31">
-        <f>SUM(K7:L7)</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+        <v>12</v>
+      </c>
+      <c r="K7" s="31">
+        <v>12</v>
+      </c>
+      <c r="L7" s="31">
+        <v>12</v>
+      </c>
       <c r="M7" s="31"/>
     </row>
     <row r="8" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="F5:F6"/>
@@ -2738,6 +2718,11 @@
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>